<commit_message>
Added PDQ drug info summary load test
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-pdq.xlsx
+++ b/test-data/webanalytics-pdq.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FB4C5685-83F0-4456-8932-3A21C8DAA510}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A8764B4E-58EF-48FF-965D-86EF0F104E72}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="PDQPage" sheetId="6" r:id="rId1"/>
-    <sheet name="RightNav" sheetId="12" r:id="rId2"/>
+    <sheet name="PDQCisPage" sheetId="13" r:id="rId1"/>
+    <sheet name="PDQDrugPage" sheetId="6" r:id="rId2"/>
+    <sheet name="RightNav" sheetId="12" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
   <si>
     <t>Path</t>
   </si>
@@ -92,6 +93,18 @@
   </si>
   <si>
     <t>Ver todas las secciones</t>
+  </si>
+  <si>
+    <t>/about-cancer/treatment/drugs/acalabrutinib</t>
+  </si>
+  <si>
+    <t>/about-cancer/treatment/drugs/recombinant-HPV-quadrivalent-vaccine</t>
+  </si>
+  <si>
+    <t>/about-cancer/treatment/drugs/sorafenibtosylate</t>
+  </si>
+  <si>
+    <t>PDQ Drug Info Summary</t>
   </si>
 </sst>
 </file>
@@ -457,11 +470,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB14744-CC2D-4AE2-9979-BD0B9D0ED780}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40CEE14B-5FDD-4B42-9C47-A62A59B964A7}">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,10 +570,62 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB14744-CC2D-4AE2-9979-BD0B9D0ED780}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="79.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCC0462B-8C8A-4BA3-9278-409F1703EE77}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed bad pdq link
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-pdq.xlsx
+++ b/test-data/webanalytics-pdq.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A8764B4E-58EF-48FF-965D-86EF0F104E72}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{22B1D371-57E9-4D9A-960D-B1FAA9C72DCE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PDQCisPage" sheetId="13" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
   <si>
     <t>Path</t>
   </si>
@@ -50,18 +50,12 @@
     <t>/types/lung/hp/lung-prevention-pdq#link/_225_toc</t>
   </si>
   <si>
-    <t>/espanol/cancer/deteccion/aspectos-generales-deteccion-paciente-pdq</t>
-  </si>
-  <si>
     <t>/espanol/cancer/deteccion/aspectos-generales-deteccion-paciente-pdq#section/all</t>
   </si>
   <si>
     <t>/espanol/cancer/deteccion/aspectos-generales-deteccion-paciente-pdq#section/_149</t>
   </si>
   <si>
-    <t>/espanol/cancer/deteccion/aspectos-generales-deteccion-paciente-pdq#link/_8</t>
-  </si>
-  <si>
     <t>PDQ Cancer Info Summary</t>
   </si>
   <si>
@@ -105,6 +99,9 @@
   </si>
   <si>
     <t>PDQ Drug Info Summary</t>
+  </si>
+  <si>
+    <t>/espanol/cancer/deteccion/aspectos-generales-deteccion-paciente-pdq#link/_AboutThis_5_toc</t>
   </si>
 </sst>
 </file>
@@ -471,15 +468,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40CEE14B-5FDD-4B42-9C47-A62A59B964A7}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="79.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="88.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -496,39 +493,39 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -536,7 +533,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -544,23 +541,15 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -573,7 +562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB14744-CC2D-4AE2-9979-BD0B9D0ED780}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -593,26 +582,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
         <v>23</v>
-      </c>
-      <c r="B3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -641,10 +630,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -652,10 +641,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
         <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -663,10 +652,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -674,10 +663,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -685,10 +674,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed actions from PDQcis click
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-pdq.xlsx
+++ b/test-data/webanalytics-pdq.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{22B1D371-57E9-4D9A-960D-B1FAA9C72DCE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{10E203BD-9F37-445B-9033-1E8002642586}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PDQCisPage" sheetId="13" r:id="rId1"/>
@@ -470,7 +470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40CEE14B-5FDD-4B42-9C47-A62A59B964A7}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -614,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCC0462B-8C8A-4BA3-9278-409F1703EE77}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed PDQ link click assertions & double-beacon issue
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-pdq.xlsx
+++ b/test-data/webanalytics-pdq.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{10E203BD-9F37-445B-9033-1E8002642586}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5407AFC0-A362-4B25-ACBF-C657CE637DD1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="PDQCisPage" sheetId="13" r:id="rId1"/>
     <sheet name="PDQDrugPage" sheetId="6" r:id="rId2"/>
     <sheet name="RightNav" sheetId="12" r:id="rId3"/>
+    <sheet name="PatientHPToggle" sheetId="14" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
   <si>
     <t>Path</t>
   </si>
@@ -59,9 +60,6 @@
     <t>PDQ Cancer Info Summary</t>
   </si>
   <si>
-    <t>SectionName</t>
-  </si>
-  <si>
     <t>Descripción de las pruebas</t>
   </si>
   <si>
@@ -71,21 +69,6 @@
     <t>Description of the Evidence</t>
   </si>
   <si>
-    <t>PageDetail</t>
-  </si>
-  <si>
-    <t>www.cancer.gov/types/lung/hp/lung-prevention-pdq/description of the evidence</t>
-  </si>
-  <si>
-    <t>www.cancer.gov/types/lung/hp/lung-prevention-pdq</t>
-  </si>
-  <si>
-    <t>www.cancer.gov/espanol/tipos/pulmon/pro/prevencion-pulmon-pdq/descripción de las pruebas</t>
-  </si>
-  <si>
-    <t>www.cancer.gov/espanol/tipos/pulmon/pro/prevencion-pulmon-pdq</t>
-  </si>
-  <si>
     <t>Ver todas las secciones</t>
   </si>
   <si>
@@ -102,6 +85,33 @@
   </si>
   <si>
     <t>/espanol/cancer/deteccion/aspectos-generales-deteccion-paciente-pdq#link/_AboutThis_5_toc</t>
+  </si>
+  <si>
+    <t>LinkText</t>
+  </si>
+  <si>
+    <t>/espanol/cancer/causas-prevencion/aspectos-generales-prevencion-paciente-pdq</t>
+  </si>
+  <si>
+    <t>vaya a la versión para profesionales de salud</t>
+  </si>
+  <si>
+    <t>/espanol/cancer/causas-prevencion/aspectos-generales-prevencion-pro-pdq</t>
+  </si>
+  <si>
+    <t>vaya a la versión para pacientes</t>
+  </si>
+  <si>
+    <t>/about-cancer/causes-prevention/hp-prevention-overview-pdq</t>
+  </si>
+  <si>
+    <t>go to patient version</t>
+  </si>
+  <si>
+    <t>/about-cancer/causes-prevention/patient-prevention-overview-pdq</t>
+  </si>
+  <si>
+    <t>go to health professional version</t>
   </si>
 </sst>
 </file>
@@ -546,7 +556,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
@@ -562,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB14744-CC2D-4AE2-9979-BD0B9D0ED780}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,26 +592,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -612,7 +622,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCC0462B-8C8A-4BA3-9278-409F1703EE77}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
@@ -620,64 +630,107 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="79.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="89.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{334744A9-1ABB-469B-B994-458EBBB5A6B3}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="76.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C5" t="s">
-        <v>18</v>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>